<commit_message>
Added Super Bowl VIII Forecast
</commit_message>
<xml_diff>
--- a/NFL2018/Validation/ValidationData.xlsx
+++ b/NFL2018/Validation/ValidationData.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2018\Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5973444-2C75-4396-B3D8-957D29814F3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620B14A-EA07-4FE9-A9F6-6AC53C5080F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="37">
   <si>
     <t>Team</t>
   </si>
@@ -982,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X497"/>
+  <dimension ref="A1:X501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E483" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K487" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A498" sqref="A498"/>
+      <selection pane="bottomRight" activeCell="W502" sqref="W502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34528,7 +34535,7 @@
         <v>32</v>
       </c>
       <c r="C448" t="str">
-        <f t="shared" ref="C448:C496" si="44">B449</f>
+        <f t="shared" ref="C448:C500" si="44">B449</f>
         <v>DEN</v>
       </c>
       <c r="D448" s="4">
@@ -36553,7 +36560,7 @@
         <v>25</v>
       </c>
       <c r="C475" t="str">
-        <f t="shared" ref="C475:C497" si="45">B474</f>
+        <f t="shared" ref="C475:C501" si="45">B474</f>
         <v>LAR</v>
       </c>
       <c r="D475" s="4">
@@ -38268,6 +38275,306 @@
       </c>
       <c r="X497" s="2">
         <v>14</v>
+      </c>
+    </row>
+    <row r="498" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A498">
+        <v>18</v>
+      </c>
+      <c r="B498" t="s">
+        <v>23</v>
+      </c>
+      <c r="C498" t="str">
+        <f t="shared" si="44"/>
+        <v>LAR</v>
+      </c>
+      <c r="D498" s="4">
+        <v>31.4199085160183</v>
+      </c>
+      <c r="E498" s="2">
+        <v>10</v>
+      </c>
+      <c r="F498" s="2">
+        <v>14</v>
+      </c>
+      <c r="G498" s="2">
+        <v>17</v>
+      </c>
+      <c r="H498" s="2">
+        <v>20</v>
+      </c>
+      <c r="I498" s="2">
+        <v>21</v>
+      </c>
+      <c r="J498" s="2">
+        <v>23</v>
+      </c>
+      <c r="K498" s="2">
+        <v>24</v>
+      </c>
+      <c r="L498" s="2">
+        <v>27</v>
+      </c>
+      <c r="M498" s="2">
+        <v>28</v>
+      </c>
+      <c r="N498" s="2">
+        <v>30</v>
+      </c>
+      <c r="O498" s="2">
+        <v>32</v>
+      </c>
+      <c r="P498" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q498" s="2">
+        <v>36</v>
+      </c>
+      <c r="R498" s="2">
+        <v>38</v>
+      </c>
+      <c r="S498" s="2">
+        <v>41</v>
+      </c>
+      <c r="T498" s="2">
+        <v>43</v>
+      </c>
+      <c r="U498" s="2">
+        <v>46</v>
+      </c>
+      <c r="V498" s="2">
+        <v>50</v>
+      </c>
+      <c r="W498" s="2">
+        <v>57</v>
+      </c>
+      <c r="X498" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="499" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A499">
+        <v>18</v>
+      </c>
+      <c r="B499" t="s">
+        <v>27</v>
+      </c>
+      <c r="C499" t="str">
+        <f t="shared" si="45"/>
+        <v>NO</v>
+      </c>
+      <c r="D499" s="4">
+        <v>30.342547531490489</v>
+      </c>
+      <c r="E499" s="2">
+        <v>10</v>
+      </c>
+      <c r="F499" s="2">
+        <v>13</v>
+      </c>
+      <c r="G499" s="2">
+        <v>16</v>
+      </c>
+      <c r="H499" s="2">
+        <v>18</v>
+      </c>
+      <c r="I499" s="2">
+        <v>20</v>
+      </c>
+      <c r="J499" s="2">
+        <v>22</v>
+      </c>
+      <c r="K499" s="2">
+        <v>24</v>
+      </c>
+      <c r="L499" s="2">
+        <v>26</v>
+      </c>
+      <c r="M499" s="2">
+        <v>27</v>
+      </c>
+      <c r="N499" s="2">
+        <v>29</v>
+      </c>
+      <c r="O499" s="2">
+        <v>31</v>
+      </c>
+      <c r="P499" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q499" s="2">
+        <v>35</v>
+      </c>
+      <c r="R499" s="2">
+        <v>37</v>
+      </c>
+      <c r="S499" s="2">
+        <v>39</v>
+      </c>
+      <c r="T499" s="2">
+        <v>42</v>
+      </c>
+      <c r="U499" s="2">
+        <v>45</v>
+      </c>
+      <c r="V499" s="2">
+        <v>49</v>
+      </c>
+      <c r="W499" s="2">
+        <v>55</v>
+      </c>
+      <c r="X499" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="500" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A500">
+        <v>18</v>
+      </c>
+      <c r="B500" t="s">
+        <v>16</v>
+      </c>
+      <c r="C500" t="str">
+        <f t="shared" si="44"/>
+        <v>NE</v>
+      </c>
+      <c r="D500" s="4">
+        <v>33.29916054016789</v>
+      </c>
+      <c r="E500" s="2">
+        <v>10</v>
+      </c>
+      <c r="F500" s="2">
+        <v>14</v>
+      </c>
+      <c r="G500" s="2">
+        <v>17</v>
+      </c>
+      <c r="H500" s="2">
+        <v>21</v>
+      </c>
+      <c r="I500" s="2">
+        <v>23</v>
+      </c>
+      <c r="J500" s="2">
+        <v>24</v>
+      </c>
+      <c r="K500" s="2">
+        <v>27</v>
+      </c>
+      <c r="L500" s="2">
+        <v>28</v>
+      </c>
+      <c r="M500" s="2">
+        <v>31</v>
+      </c>
+      <c r="N500" s="2">
+        <v>31</v>
+      </c>
+      <c r="O500" s="2">
+        <v>34</v>
+      </c>
+      <c r="P500" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q500" s="2">
+        <v>38</v>
+      </c>
+      <c r="R500" s="2">
+        <v>41</v>
+      </c>
+      <c r="S500" s="2">
+        <v>42</v>
+      </c>
+      <c r="T500" s="2">
+        <v>45</v>
+      </c>
+      <c r="U500" s="2">
+        <v>48</v>
+      </c>
+      <c r="V500" s="2">
+        <v>52</v>
+      </c>
+      <c r="W500" s="2">
+        <v>59</v>
+      </c>
+      <c r="X500" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="501" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A501">
+        <v>18</v>
+      </c>
+      <c r="B501" t="s">
+        <v>29</v>
+      </c>
+      <c r="C501" t="str">
+        <f t="shared" si="45"/>
+        <v>KC</v>
+      </c>
+      <c r="D501" s="4">
+        <v>29.888306822338631</v>
+      </c>
+      <c r="E501" s="2">
+        <v>10</v>
+      </c>
+      <c r="F501" s="2">
+        <v>13</v>
+      </c>
+      <c r="G501" s="2">
+        <v>16</v>
+      </c>
+      <c r="H501" s="2">
+        <v>17</v>
+      </c>
+      <c r="I501" s="2">
+        <v>20</v>
+      </c>
+      <c r="J501" s="2">
+        <v>21</v>
+      </c>
+      <c r="K501" s="2">
+        <v>24</v>
+      </c>
+      <c r="L501" s="2">
+        <v>26</v>
+      </c>
+      <c r="M501" s="2">
+        <v>27</v>
+      </c>
+      <c r="N501" s="2">
+        <v>28</v>
+      </c>
+      <c r="O501" s="2">
+        <v>31</v>
+      </c>
+      <c r="P501" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q501" s="2">
+        <v>34</v>
+      </c>
+      <c r="R501" s="2">
+        <v>37</v>
+      </c>
+      <c r="S501" s="2">
+        <v>38</v>
+      </c>
+      <c r="T501" s="2">
+        <v>41</v>
+      </c>
+      <c r="U501" s="2">
+        <v>44</v>
+      </c>
+      <c r="V501" s="2">
+        <v>48</v>
+      </c>
+      <c r="W501" s="2">
+        <v>55</v>
+      </c>
+      <c r="X501" s="2">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2019 Week 8 NFL forecasts
</commit_message>
<xml_diff>
--- a/NFL2018/Validation/ValidationData.xlsx
+++ b/NFL2018/Validation/ValidationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2018\Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620B14A-EA07-4FE9-A9F6-6AC53C5080F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34FC22A-2444-43CD-83B6-804FEF16E6DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="37">
   <si>
     <t>Team</t>
   </si>
@@ -989,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X501"/>
+  <dimension ref="A1:X503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K487" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E486" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W502" sqref="W502"/>
+      <selection pane="bottomRight" activeCell="A504" sqref="A504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34535,7 +34535,7 @@
         <v>32</v>
       </c>
       <c r="C448" t="str">
-        <f t="shared" ref="C448:C500" si="44">B449</f>
+        <f t="shared" ref="C448:C502" si="44">B449</f>
         <v>DEN</v>
       </c>
       <c r="D448" s="4">
@@ -36560,7 +36560,7 @@
         <v>25</v>
       </c>
       <c r="C475" t="str">
-        <f t="shared" ref="C475:C501" si="45">B474</f>
+        <f t="shared" ref="C475:C503" si="45">B474</f>
         <v>LAR</v>
       </c>
       <c r="D475" s="4">
@@ -38575,6 +38575,156 @@
       </c>
       <c r="X501" s="2">
         <v>37</v>
+      </c>
+    </row>
+    <row r="502" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A502">
+        <v>18</v>
+      </c>
+      <c r="B502" t="s">
+        <v>29</v>
+      </c>
+      <c r="C502" t="str">
+        <f>B503</f>
+        <v>LAR</v>
+      </c>
+      <c r="D502" s="4">
+        <v>29.302967339406528</v>
+      </c>
+      <c r="E502" s="2">
+        <v>10</v>
+      </c>
+      <c r="F502" s="2">
+        <v>13</v>
+      </c>
+      <c r="G502" s="2">
+        <v>16</v>
+      </c>
+      <c r="H502" s="2">
+        <v>17</v>
+      </c>
+      <c r="I502" s="2">
+        <v>20</v>
+      </c>
+      <c r="J502" s="2">
+        <v>21</v>
+      </c>
+      <c r="K502" s="2">
+        <v>23</v>
+      </c>
+      <c r="L502" s="2">
+        <v>24</v>
+      </c>
+      <c r="M502" s="2">
+        <v>27</v>
+      </c>
+      <c r="N502" s="2">
+        <v>28</v>
+      </c>
+      <c r="O502" s="2">
+        <v>30</v>
+      </c>
+      <c r="P502" s="2">
+        <v>31</v>
+      </c>
+      <c r="Q502" s="2">
+        <v>34</v>
+      </c>
+      <c r="R502" s="2">
+        <v>35</v>
+      </c>
+      <c r="S502" s="2">
+        <v>38</v>
+      </c>
+      <c r="T502" s="2">
+        <v>41</v>
+      </c>
+      <c r="U502" s="2">
+        <v>44</v>
+      </c>
+      <c r="V502" s="2">
+        <v>48</v>
+      </c>
+      <c r="W502" s="2">
+        <v>54</v>
+      </c>
+      <c r="X502" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="503" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A503">
+        <v>18</v>
+      </c>
+      <c r="B503" t="s">
+        <v>27</v>
+      </c>
+      <c r="C503" t="str">
+        <f t="shared" si="45"/>
+        <v>NE</v>
+      </c>
+      <c r="D503" s="4">
+        <v>30.216897156620568</v>
+      </c>
+      <c r="E503" s="2">
+        <v>10</v>
+      </c>
+      <c r="F503" s="2">
+        <v>13</v>
+      </c>
+      <c r="G503" s="2">
+        <v>16</v>
+      </c>
+      <c r="H503" s="2">
+        <v>19</v>
+      </c>
+      <c r="I503" s="2">
+        <v>20</v>
+      </c>
+      <c r="J503" s="2">
+        <v>23</v>
+      </c>
+      <c r="K503" s="2">
+        <v>24</v>
+      </c>
+      <c r="L503" s="2">
+        <v>26</v>
+      </c>
+      <c r="M503" s="2">
+        <v>27</v>
+      </c>
+      <c r="N503" s="2">
+        <v>29</v>
+      </c>
+      <c r="O503" s="2">
+        <v>31</v>
+      </c>
+      <c r="P503" s="2">
+        <v>33</v>
+      </c>
+      <c r="Q503" s="2">
+        <v>34</v>
+      </c>
+      <c r="R503" s="2">
+        <v>37</v>
+      </c>
+      <c r="S503" s="2">
+        <v>39</v>
+      </c>
+      <c r="T503" s="2">
+        <v>41</v>
+      </c>
+      <c r="U503" s="2">
+        <v>44</v>
+      </c>
+      <c r="V503" s="2">
+        <v>48</v>
+      </c>
+      <c r="W503" s="2">
+        <v>54</v>
+      </c>
+      <c r="X503" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>